<commit_message>
Nieuwe GDD Graag lezen!
Zou mij hartje een hoop plezier geven als jullie de nieuwe gdd lezen.
MAAR 2K worden.
Plis, voor iedere gelezen GDD kunt u een afrikaantje schoenen geven
</commit_message>
<xml_diff>
--- a/Planning/Planning_GL3.xlsx
+++ b/Planning/Planning_GL3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Deltion\Derde Jaar\Gamelab_3\Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Deltion\Derde Jaar\GameLab 3 Mack\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,8 @@
   <sheets>
     <sheet name="GEHEEL" sheetId="1" r:id="rId1"/>
     <sheet name="Artist" sheetId="2" r:id="rId2"/>
-    <sheet name="Script" sheetId="3" r:id="rId3"/>
+    <sheet name="Volgorde" sheetId="4" r:id="rId3"/>
+    <sheet name="Script" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="167">
   <si>
     <t>Planning</t>
   </si>
@@ -485,13 +486,55 @@
   </si>
   <si>
     <t>Week 51</t>
+  </si>
+  <si>
+    <t>Le_Arena_001</t>
+  </si>
+  <si>
+    <t>MA_Sacrifial_003</t>
+  </si>
+  <si>
+    <t>WE_Spear_003</t>
+  </si>
+  <si>
+    <t>WE_Spear_004</t>
+  </si>
+  <si>
+    <t>Wat we nog moeten</t>
+  </si>
+  <si>
+    <t>Wat we al hebben</t>
+  </si>
+  <si>
+    <t>EN_Chest_001</t>
+  </si>
+  <si>
+    <t>WE_Sword_004</t>
+  </si>
+  <si>
+    <t>WE_Bolt_002</t>
+  </si>
+  <si>
+    <t>MA_Illusory_001</t>
+  </si>
+  <si>
+    <t>MA_Illusory_002</t>
+  </si>
+  <si>
+    <t>2DE_HUD_Gold</t>
+  </si>
+  <si>
+    <t>EN_Chest_002</t>
+  </si>
+  <si>
+    <t>Bu_Destructible_001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -520,8 +563,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -549,6 +600,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -593,7 +650,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -608,6 +665,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -2295,8 +2354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2345,7 +2404,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>49</v>
+        <v>144</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>50</v>
@@ -2398,7 +2457,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>49</v>
+        <v>144</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>50</v>
@@ -2419,7 +2478,7 @@
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4"/>
       <c r="C10" s="4" t="s">
-        <v>51</v>
+        <v>155</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>130</v>
@@ -2435,7 +2494,7 @@
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
-        <v>52</v>
+        <v>156</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
@@ -2463,7 +2522,7 @@
         <v>15</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>49</v>
+        <v>144</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>50</v>
@@ -2528,7 +2587,7 @@
         <v>22</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>49</v>
+        <v>144</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>50</v>
@@ -2548,14 +2607,12 @@
     </row>
     <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="4" t="s">
-        <v>67</v>
+        <v>154</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>94</v>
-      </c>
+      <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4" t="s">
         <v>112</v>
@@ -2563,24 +2620,18 @@
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="4" t="s">
-        <v>66</v>
-      </c>
+      <c r="B19" s="4"/>
       <c r="C19" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>95</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="4"/>
-      <c r="C20" s="4" t="s">
-        <v>91</v>
-      </c>
+      <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -2591,10 +2642,10 @@
         <v>23</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>50</v>
+        <v>153</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>65</v>
@@ -2603,25 +2654,21 @@
         <v>122</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>115</v>
+        <v>153</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>136</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="4"/>
-      <c r="C22" s="4" t="s">
-        <v>92</v>
-      </c>
+      <c r="C22" s="4"/>
       <c r="D22" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
-      <c r="G22" s="4" t="s">
-        <v>138</v>
-      </c>
+      <c r="G22" s="4"/>
     </row>
     <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="4"/>
@@ -2629,9 +2676,7 @@
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
-      <c r="G23" s="4" t="s">
-        <v>137</v>
-      </c>
+      <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="4"/>
@@ -2646,31 +2691,29 @@
         <v>24</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>50</v>
+        <v>153</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="E25" s="9" t="s">
         <v>123</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>115</v>
+        <v>153</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>150</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="4"/>
-      <c r="C26" s="4" t="s">
-        <v>92</v>
-      </c>
+      <c r="C26" s="4"/>
       <c r="D26" s="4" t="s">
-        <v>98</v>
+        <v>141</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -2680,7 +2723,7 @@
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4" t="s">
-        <v>99</v>
+        <v>145</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
@@ -2803,50 +2846,56 @@
         <v>33</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>50</v>
+        <v>153</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="E34" s="8" t="s">
         <v>124</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>114</v>
+        <v>153</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>150</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
+        <v>160</v>
+      </c>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>120</v>
+      </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
     </row>
     <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="4" t="s">
-        <v>70</v>
-      </c>
+      <c r="B36" s="4"/>
       <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
+      <c r="D36" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>164</v>
+      </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
     </row>
     <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
+      <c r="D37" s="4" t="s">
+        <v>145</v>
+      </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
@@ -2856,52 +2905,50 @@
         <v>34</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>50</v>
+        <v>153</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>125</v>
+        <v>164</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="G38" s="9" t="s">
-        <v>150</v>
+        <v>153</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4" t="s">
-        <v>117</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F39" s="4"/>
       <c r="G39" s="4"/>
     </row>
     <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="4" t="s">
-        <v>71</v>
-      </c>
+      <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
+      <c r="E40" s="4" t="s">
+        <v>128</v>
+      </c>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
     </row>
     <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="4" t="s">
-        <v>72</v>
-      </c>
+      <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
@@ -2913,58 +2960,54 @@
         <v>35</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="D42" s="8"/>
+        <v>101</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>94</v>
+      </c>
       <c r="E42" s="8" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="F42" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="G42" s="9" t="s">
-        <v>141</v>
+      <c r="G42" s="8" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="4" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D43" s="4"/>
+        <v>103</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>96</v>
+      </c>
       <c r="E43" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="G43" s="4" t="s">
-        <v>142</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="G43" s="4"/>
     </row>
     <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="4" t="s">
-        <v>75</v>
-      </c>
+      <c r="B44" s="4"/>
       <c r="C44" s="4" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
-      <c r="G44" s="4" t="s">
-        <v>143</v>
-      </c>
+      <c r="G44" s="4"/>
     </row>
     <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="4" t="s">
-        <v>76</v>
-      </c>
+      <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
@@ -2976,47 +3019,49 @@
         <v>77</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="D46" s="8"/>
+        <v>101</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>96</v>
+      </c>
       <c r="E46" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F46" s="8" t="s">
         <v>116</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>144</v>
+        <v>166</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="4"/>
+      <c r="B47" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="C47" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G47" s="4"/>
+    </row>
+    <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C48" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="4"/>
-      <c r="C48" s="4" t="s">
-        <v>105</v>
-      </c>
       <c r="D48" s="4"/>
-      <c r="E48" s="4" t="s">
-        <v>129</v>
-      </c>
+      <c r="E48" s="4"/>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
     </row>
@@ -3033,40 +3078,46 @@
         <v>78</v>
       </c>
       <c r="B50" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="G50" s="9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C50" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="D50" s="8"/>
-      <c r="E50" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="F50" s="8"/>
-      <c r="G50" s="9" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="4"/>
-      <c r="C51" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="D51" s="4"/>
-      <c r="E51" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="F51" s="4"/>
-      <c r="G51" s="4" t="s">
-        <v>145</v>
-      </c>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G51" s="4"/>
     </row>
     <row r="52" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
-      <c r="F52" s="4"/>
+      <c r="F52" s="4" t="s">
+        <v>109</v>
+      </c>
       <c r="G52" s="4"/>
     </row>
     <row r="53" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3074,7 +3125,9 @@
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
-      <c r="F53" s="4"/>
+      <c r="F53" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="G53" s="4"/>
     </row>
     <row r="54" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3082,32 +3135,46 @@
         <v>79</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
+        <v>85</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>98</v>
+      </c>
       <c r="E54" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="F54" s="8"/>
-      <c r="G54" s="8" t="s">
-        <v>146</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="G54" s="8"/>
     </row>
     <row r="55" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="4"/>
+      <c r="B55" s="4" t="s">
+        <v>69</v>
+      </c>
       <c r="C55" s="4"/>
-      <c r="D55" s="4"/>
+      <c r="D55" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="E55" s="4"/>
-      <c r="F55" s="4"/>
+      <c r="F55" s="4" t="s">
+        <v>109</v>
+      </c>
       <c r="G55" s="4"/>
     </row>
     <row r="56" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="4"/>
+      <c r="B56" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
-      <c r="F56" s="4"/>
+      <c r="F56" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="G56" s="4"/>
     </row>
     <row r="57" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3123,24 +3190,34 @@
         <v>80</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
+        <v>76</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>99</v>
+      </c>
       <c r="E58" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="F58" s="8"/>
-      <c r="G58" s="8" t="s">
-        <v>147</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="G58" s="8"/>
     </row>
     <row r="59" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="4"/>
-      <c r="C59" s="4"/>
-      <c r="D59" s="4"/>
+      <c r="C59" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="E59" s="4"/>
-      <c r="F59" s="4"/>
+      <c r="F59" s="4" t="s">
+        <v>109</v>
+      </c>
       <c r="G59" s="4"/>
     </row>
     <row r="60" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3148,7 +3225,9 @@
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
-      <c r="F60" s="4"/>
+      <c r="F60" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="G60" s="4"/>
     </row>
     <row r="61" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3164,14 +3243,18 @@
         <v>81</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C62" s="8"/>
-      <c r="D62" s="8"/>
+        <v>76</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>95</v>
+      </c>
       <c r="E62" s="8"/>
       <c r="F62" s="8"/>
       <c r="G62" s="8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3180,9 +3263,7 @@
       <c r="D63" s="4"/>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
-      <c r="G63" s="4" t="s">
-        <v>149</v>
-      </c>
+      <c r="G63" s="4"/>
     </row>
     <row r="64" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B64" s="4"/>
@@ -3204,9 +3285,7 @@
       <c r="A66" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="B66" s="8" t="s">
-        <v>75</v>
-      </c>
+      <c r="B66" s="8"/>
       <c r="C66" s="8"/>
       <c r="D66" s="8"/>
       <c r="E66" s="8"/>
@@ -3214,16 +3293,12 @@
       <c r="G66" s="8"/>
     </row>
     <row r="67" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="4" t="s">
-        <v>76</v>
-      </c>
+      <c r="B67" s="4"/>
       <c r="C67" s="4"/>
       <c r="D67" s="4"/>
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
-      <c r="G67" s="4" t="s">
-        <v>140</v>
-      </c>
+      <c r="G67" s="4"/>
     </row>
     <row r="68" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="4"/>
@@ -3231,9 +3306,7 @@
       <c r="D68" s="4"/>
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
-      <c r="G68" s="4" t="s">
-        <v>139</v>
-      </c>
+      <c r="G68" s="4"/>
     </row>
     <row r="69" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B69" s="4"/>
@@ -3257,6 +3330,188 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="14" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E49"/>
   <sheetViews>

</xml_diff>

<commit_message>
Planning even goed verandert
Want ik weet wel hoe da gaat. Oh en was te vergeten te melden dat Trello
ook geupdate is. Kevin moet nog wel even op de Trello komen.
</commit_message>
<xml_diff>
--- a/Planning/Planning_GL3.xlsx
+++ b/Planning/Planning_GL3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17220" windowHeight="9690" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17220" windowHeight="9690"/>
   </bookViews>
   <sheets>
     <sheet name="GEHEEL" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="150">
   <si>
     <t>Planning</t>
   </si>
@@ -176,9 +176,6 @@
     <t>Networking</t>
   </si>
   <si>
-    <t>NP_Turret_001</t>
-  </si>
-  <si>
     <t>LV_MOBA_001</t>
   </si>
   <si>
@@ -227,21 +224,6 @@
     <t>AR_LightArmourSet_001</t>
   </si>
   <si>
-    <t>BU_Homebase_001</t>
-  </si>
-  <si>
-    <t>NP_Inhibitor_001</t>
-  </si>
-  <si>
-    <t>WE_Sword_005</t>
-  </si>
-  <si>
-    <t>WE_Club_001</t>
-  </si>
-  <si>
-    <t>WE_Club_002</t>
-  </si>
-  <si>
     <t>WE_Bow_001</t>
   </si>
   <si>
@@ -275,12 +257,6 @@
     <t>Week 50</t>
   </si>
   <si>
-    <t>NP_SiegeUnit_001</t>
-  </si>
-  <si>
-    <t>NP_Magic_Evocation_001</t>
-  </si>
-  <si>
     <t>AR_HeavyArmourSet_001</t>
   </si>
   <si>
@@ -302,12 +278,6 @@
     <t>PC_Female_001</t>
   </si>
   <si>
-    <t>BU_Shop_Siege_001</t>
-  </si>
-  <si>
-    <t>EN_Jungle_000</t>
-  </si>
-  <si>
     <t>WE_Greatsword_001</t>
   </si>
   <si>
@@ -347,12 +317,6 @@
     <t>MA_Imperial_003</t>
   </si>
   <si>
-    <t>MA_Illosury_001</t>
-  </si>
-  <si>
-    <t>MA_Illosury_002</t>
-  </si>
-  <si>
     <t>WE_Barbell_001</t>
   </si>
   <si>
@@ -368,15 +332,6 @@
     <t>IT_Potion_Stamina_001</t>
   </si>
   <si>
-    <t>EN_Texture_Jungle_001</t>
-  </si>
-  <si>
-    <t>EN_Texture_Lane_001</t>
-  </si>
-  <si>
-    <t>BU_Shop_Normal_001</t>
-  </si>
-  <si>
     <t>AR_MediumArmourSet_001</t>
   </si>
   <si>
@@ -407,12 +362,6 @@
     <t>AR_LightArmourSet_002</t>
   </si>
   <si>
-    <t>BU_Magic_001</t>
-  </si>
-  <si>
-    <t>BU_Magic_002</t>
-  </si>
-  <si>
     <t>MA_Invocation_002</t>
   </si>
   <si>
@@ -422,9 +371,6 @@
     <t>NP_Min_Melee_001</t>
   </si>
   <si>
-    <t>NP_Min_Ranged_001</t>
-  </si>
-  <si>
     <t>NP_Creep_Melee_001</t>
   </si>
   <si>
@@ -437,15 +383,6 @@
     <t>NP_Creep_Super_001</t>
   </si>
   <si>
-    <t>NP_Magic_Evocation_002</t>
-  </si>
-  <si>
-    <t>IT_Buff_Strength_001</t>
-  </si>
-  <si>
-    <t>IT_Buff_HealthRegen_001</t>
-  </si>
-  <si>
     <t>WE_Dagger_001</t>
   </si>
   <si>
@@ -458,28 +395,7 @@
     <t>WE_Shield_Medium_001</t>
   </si>
   <si>
-    <t>WE_Shield_Large_001</t>
-  </si>
-  <si>
     <t>MA_Evocation_001</t>
-  </si>
-  <si>
-    <t>MA_Evocation_002</t>
-  </si>
-  <si>
-    <t>MA_Sacrifial_001</t>
-  </si>
-  <si>
-    <t>MA_Sacrifial_002</t>
-  </si>
-  <si>
-    <t>MA_Abjuration_001</t>
-  </si>
-  <si>
-    <t>MA_Abjuration_002</t>
-  </si>
-  <si>
-    <t>NP_Boss_002</t>
   </si>
   <si>
     <t>Vakantie</t>
@@ -982,7 +898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L70"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:G70"/>
     </sheetView>
   </sheetViews>
@@ -1052,22 +968,22 @@
         <v>13</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>50</v>
-      </c>
       <c r="D5" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E5" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>56</v>
-      </c>
       <c r="G5" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>13</v>
@@ -1091,7 +1007,7 @@
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G6" s="4"/>
       <c r="I6" s="6" t="s">
@@ -1109,7 +1025,7 @@
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G7" s="4"/>
       <c r="I7" s="6"/>
@@ -1125,7 +1041,7 @@
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G8" s="4"/>
       <c r="I8" s="6"/>
@@ -1138,28 +1054,28 @@
         <v>14</v>
       </c>
       <c r="B9" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>50</v>
-      </c>
       <c r="D9" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>54</v>
-      </c>
       <c r="F9" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>14</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J9" s="8" t="s">
         <v>18</v>
@@ -1174,16 +1090,16 @@
     <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4"/>
       <c r="C10" s="4" t="s">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G10" s="4"/>
       <c r="I10" s="6"/>
@@ -1196,14 +1112,14 @@
     <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
-        <v>52</v>
+        <v>127</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G11" s="4"/>
       <c r="I11" s="6"/>
@@ -1218,10 +1134,10 @@
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G12" s="4"/>
       <c r="I12" s="6"/>
@@ -1234,28 +1150,28 @@
         <v>15</v>
       </c>
       <c r="B13" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>50</v>
-      </c>
       <c r="D13" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J13" s="8" t="s">
         <v>18</v>
@@ -1270,19 +1186,19 @@
     <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="4"/>
       <c r="C14" s="4" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
@@ -1296,15 +1212,15 @@
     <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
@@ -1316,7 +1232,7 @@
     <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="4"/>
       <c r="C16" s="4" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
@@ -1332,28 +1248,28 @@
         <v>22</v>
       </c>
       <c r="B17" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>50</v>
-      </c>
       <c r="D17" s="8" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>22</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J17" s="8" t="s">
         <v>25</v>
@@ -1367,17 +1283,15 @@
     </row>
     <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="4" t="s">
-        <v>67</v>
+        <v>149</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>94</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="G18" s="4"/>
       <c r="I18" s="6"/>
@@ -1392,15 +1306,11 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="4" t="s">
-        <v>66</v>
-      </c>
+      <c r="B19" s="4"/>
       <c r="C19" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>95</v>
-      </c>
+      <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -1411,9 +1321,7 @@
     </row>
     <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="4"/>
-      <c r="C20" s="4" t="s">
-        <v>91</v>
-      </c>
+      <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -1428,28 +1336,28 @@
         <v>23</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>50</v>
+        <v>148</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>115</v>
+        <v>148</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>136</v>
+        <v>81</v>
       </c>
       <c r="H21" s="7" t="s">
         <v>23</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J21" s="8" t="s">
         <v>27</v>
@@ -1463,17 +1371,13 @@
     </row>
     <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="4"/>
-      <c r="C22" s="4" t="s">
-        <v>92</v>
-      </c>
+      <c r="C22" s="4"/>
       <c r="D22" s="4" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
-      <c r="G22" s="4" t="s">
-        <v>138</v>
-      </c>
+      <c r="G22" s="4"/>
       <c r="I22" s="6"/>
       <c r="J22" s="6" t="s">
         <v>28</v>
@@ -1491,9 +1395,7 @@
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
-      <c r="G23" s="4" t="s">
-        <v>137</v>
-      </c>
+      <c r="G23" s="4"/>
       <c r="I23" s="6"/>
       <c r="J23" s="6" t="s">
         <v>29</v>
@@ -1520,28 +1422,28 @@
         <v>24</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>50</v>
+        <v>148</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>97</v>
+        <v>64</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>115</v>
+        <v>148</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>150</v>
+        <v>81</v>
       </c>
       <c r="H25" s="7" t="s">
         <v>24</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J25" s="8" t="s">
         <v>31</v>
@@ -1555,15 +1457,19 @@
     </row>
     <row r="26" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="4"/>
-      <c r="C26" s="4" t="s">
-        <v>92</v>
-      </c>
+      <c r="C26" s="4"/>
       <c r="D26" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
+        <v>137</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
@@ -1572,10 +1478,10 @@
     <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
-      <c r="D27" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4" t="s">
+        <v>139</v>
+      </c>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="I27" s="6"/>
@@ -1587,7 +1493,9 @@
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
+      <c r="E28" s="4" t="s">
+        <v>140</v>
+      </c>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="I28" s="6"/>
@@ -1600,167 +1508,167 @@
         <v>32</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="H29" s="12" t="s">
         <v>32</v>
       </c>
       <c r="I29" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="J29" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="K29" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="L29" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B30" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="J30" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="K30" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="L30" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B31" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="I31" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="J31" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="K31" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="L31" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B32" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="J32" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="K32" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="L32" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" spans="1:12" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="13"/>
       <c r="B33" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="H33" s="13"/>
       <c r="I33" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="J33" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="K33" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="L33" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1768,28 +1676,28 @@
         <v>33</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>50</v>
+        <v>148</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>114</v>
+        <v>148</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>150</v>
+        <v>81</v>
       </c>
       <c r="H34" s="7" t="s">
         <v>33</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J34" s="8" t="s">
         <v>40</v>
@@ -1803,15 +1711,19 @@
     </row>
     <row r="35" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
+        <v>131</v>
+      </c>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>139</v>
+      </c>
       <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
+      <c r="G35" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="I35" s="6"/>
       <c r="J35" s="6"/>
       <c r="K35" s="6" t="s">
@@ -1820,12 +1732,14 @@
       <c r="L35" s="6"/>
     </row>
     <row r="36" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="4" t="s">
-        <v>70</v>
-      </c>
+      <c r="B36" s="4"/>
       <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
+      <c r="D36" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>140</v>
+      </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
       <c r="I36" s="6"/>
@@ -1840,7 +1754,9 @@
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
+      <c r="E37" s="4" t="s">
+        <v>133</v>
+      </c>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
       <c r="H37"/>
@@ -1854,28 +1770,28 @@
         <v>34</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>50</v>
+        <v>148</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="G38" s="9" t="s">
-        <v>150</v>
+        <v>148</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>81</v>
       </c>
       <c r="H38" s="7" t="s">
         <v>34</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J38" s="8" t="s">
         <v>40</v>
@@ -1889,31 +1805,35 @@
     </row>
     <row r="39" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
+        <v>132</v>
+      </c>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="F39" s="4" t="s">
-        <v>117</v>
+        <v>147</v>
       </c>
       <c r="G39" s="4"/>
       <c r="I39" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J39" s="6"/>
       <c r="K39" s="6"/>
       <c r="L39" s="6"/>
     </row>
     <row r="40" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="4" t="s">
-        <v>71</v>
-      </c>
+      <c r="B40" s="4"/>
       <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
+      <c r="D40" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
       <c r="I40" s="6"/>
@@ -1923,9 +1843,7 @@
     </row>
     <row r="41" spans="1:12" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41"/>
-      <c r="B41" s="4" t="s">
-        <v>72</v>
-      </c>
+      <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
@@ -1942,20 +1860,22 @@
         <v>35</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="D42" s="8"/>
+        <v>91</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>84</v>
+      </c>
       <c r="E42" s="8" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="G42" s="9" t="s">
-        <v>141</v>
+        <v>101</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>81</v>
       </c>
       <c r="H42" s="7" t="s">
         <v>35</v>
@@ -1973,41 +1893,37 @@
     </row>
     <row r="43" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="4" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D43" s="4"/>
+        <v>93</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="E43" s="4" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="G43" s="4" t="s">
-        <v>142</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="G43" s="4"/>
       <c r="I43" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J43" s="6"/>
       <c r="K43" s="6"/>
       <c r="L43" s="6"/>
     </row>
     <row r="44" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="4" t="s">
-        <v>75</v>
-      </c>
+      <c r="B44" s="4"/>
       <c r="C44" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
-      <c r="G44" s="4" t="s">
-        <v>143</v>
-      </c>
+      <c r="G44" s="4"/>
       <c r="I44" s="6"/>
       <c r="J44" s="6"/>
       <c r="K44" s="6"/>
@@ -2015,9 +1931,7 @@
     </row>
     <row r="45" spans="1:12" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45"/>
-      <c r="B45" s="4" t="s">
-        <v>76</v>
-      </c>
+      <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
@@ -2031,26 +1945,28 @@
     </row>
     <row r="46" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="D46" s="8"/>
+        <v>91</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>86</v>
+      </c>
       <c r="E46" s="8" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="I46" s="8" t="s">
         <v>48</v>
@@ -2060,36 +1976,38 @@
       <c r="L46" s="8"/>
     </row>
     <row r="47" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="4"/>
+      <c r="B47" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="C47" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="D47" s="4"/>
+        <v>93</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="E47" s="4" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>145</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="G47" s="4"/>
       <c r="I47" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J47" s="6"/>
       <c r="K47" s="6"/>
       <c r="L47" s="6"/>
     </row>
     <row r="48" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="4"/>
+      <c r="B48" s="4" t="s">
+        <v>69</v>
+      </c>
       <c r="C48" s="4" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="D48" s="4"/>
-      <c r="E48" s="4" t="s">
-        <v>129</v>
-      </c>
+      <c r="E48" s="4"/>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
       <c r="I48" s="6"/>
@@ -2113,21 +2031,25 @@
     </row>
     <row r="50" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="D50" s="8"/>
+        <v>92</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>87</v>
+      </c>
       <c r="E50" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="F50" s="8"/>
+        <v>110</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>130</v>
+      </c>
       <c r="G50" s="9" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="H50" s="7"/>
       <c r="I50" s="7"/>
@@ -2136,25 +2058,31 @@
       <c r="L50" s="7"/>
     </row>
     <row r="51" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="4"/>
+      <c r="B51" s="4" t="s">
+        <v>69</v>
+      </c>
       <c r="C51" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="D51" s="4"/>
+        <v>95</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="E51" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="F51" s="4"/>
-      <c r="G51" s="4" t="s">
-        <v>145</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G51" s="4"/>
     </row>
     <row r="52" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
-      <c r="F52" s="4"/>
+      <c r="F52" s="4" t="s">
+        <v>97</v>
+      </c>
       <c r="G52" s="4"/>
     </row>
     <row r="53" spans="1:12" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2163,7 +2091,9 @@
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
-      <c r="F53" s="4"/>
+      <c r="F53" s="4" t="s">
+        <v>98</v>
+      </c>
       <c r="G53" s="4"/>
       <c r="H53"/>
       <c r="I53"/>
@@ -2173,19 +2103,25 @@
     </row>
     <row r="54" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
+        <v>77</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>88</v>
+      </c>
       <c r="E54" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="F54" s="8"/>
-      <c r="G54" s="8" t="s">
-        <v>146</v>
+        <v>141</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="G54" s="9" t="s">
+        <v>134</v>
       </c>
       <c r="H54" s="7"/>
       <c r="I54" s="7"/>
@@ -2195,10 +2131,18 @@
     </row>
     <row r="55" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="4"/>
-      <c r="C55" s="4"/>
-      <c r="D55" s="4"/>
-      <c r="E55" s="4"/>
-      <c r="F55" s="4"/>
+      <c r="C55" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>98</v>
+      </c>
       <c r="G55" s="4"/>
     </row>
     <row r="56" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2225,19 +2169,25 @@
     </row>
     <row r="58" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B58" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C58" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
+      <c r="D58" s="8" t="s">
+        <v>89</v>
+      </c>
       <c r="E58" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="F58" s="8"/>
-      <c r="G58" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="G58" s="9" t="s">
+        <v>134</v>
       </c>
       <c r="H58" s="7"/>
       <c r="I58" s="7"/>
@@ -2248,9 +2198,15 @@
     <row r="59" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
-      <c r="D59" s="4"/>
-      <c r="E59" s="4"/>
-      <c r="F59" s="4"/>
+      <c r="D59" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>98</v>
+      </c>
       <c r="G59" s="4"/>
     </row>
     <row r="60" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2258,7 +2214,9 @@
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
-      <c r="F60" s="4"/>
+      <c r="F60" s="4" t="s">
+        <v>102</v>
+      </c>
       <c r="G60" s="4"/>
     </row>
     <row r="61" spans="1:12" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2277,18 +2235,24 @@
     </row>
     <row r="62" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C62" s="8"/>
-      <c r="D62" s="8"/>
-      <c r="E62" s="8"/>
-      <c r="F62" s="8"/>
-      <c r="G62" s="8" t="s">
-        <v>148</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E62" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F62" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="G62" s="8"/>
       <c r="H62" s="7"/>
       <c r="I62" s="7"/>
       <c r="J62" s="7"/>
@@ -2299,11 +2263,11 @@
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
-      <c r="E63" s="4"/>
+      <c r="E63" s="4" t="s">
+        <v>144</v>
+      </c>
       <c r="F63" s="4"/>
-      <c r="G63" s="4" t="s">
-        <v>149</v>
-      </c>
+      <c r="G63" s="4"/>
     </row>
     <row r="64" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B64" s="4"/>
@@ -2323,15 +2287,17 @@
     </row>
     <row r="66" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="B66" s="8" t="s">
-        <v>75</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="B66" s="8"/>
       <c r="C66" s="8"/>
       <c r="D66" s="8"/>
-      <c r="E66" s="8"/>
-      <c r="F66" s="8"/>
+      <c r="E66" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F66" s="8" t="s">
+        <v>102</v>
+      </c>
       <c r="G66" s="8"/>
       <c r="H66" s="7"/>
       <c r="I66" s="7"/>
@@ -2340,16 +2306,12 @@
       <c r="L66" s="7"/>
     </row>
     <row r="67" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="4" t="s">
-        <v>76</v>
-      </c>
+      <c r="B67" s="4"/>
       <c r="C67" s="4"/>
       <c r="D67" s="4"/>
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
-      <c r="G67" s="4" t="s">
-        <v>140</v>
-      </c>
+      <c r="G67" s="4"/>
     </row>
     <row r="68" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="4"/>
@@ -2357,9 +2319,7 @@
       <c r="D68" s="4"/>
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
-      <c r="G68" s="4" t="s">
-        <v>139</v>
-      </c>
+      <c r="G68" s="4"/>
     </row>
     <row r="69" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B69" s="4"/>
@@ -2387,8 +2347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:G70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2437,22 +2397,22 @@
         <v>13</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E5" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>56</v>
-      </c>
       <c r="G5" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2461,7 +2421,7 @@
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G6" s="4"/>
     </row>
@@ -2471,7 +2431,7 @@
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G7" s="4"/>
     </row>
@@ -2481,7 +2441,7 @@
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G8" s="4"/>
     </row>
@@ -2490,51 +2450,51 @@
         <v>14</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>54</v>
-      </c>
       <c r="F9" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4"/>
       <c r="C10" s="4" t="s">
-        <v>154</v>
+        <v>126</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
-        <v>155</v>
+        <v>127</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G11" s="4"/>
     </row>
@@ -2543,10 +2503,10 @@
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G12" s="4"/>
     </row>
@@ -2555,60 +2515,60 @@
         <v>15</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="4"/>
       <c r="C14" s="4" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="4"/>
       <c r="C16" s="4" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
@@ -2620,42 +2580,42 @@
         <v>22</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="4" t="s">
-        <v>177</v>
+        <v>149</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="4"/>
       <c r="C19" s="4" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
@@ -2675,29 +2635,29 @@
         <v>23</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
@@ -2724,38 +2684,38 @@
         <v>24</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4" t="s">
-        <v>165</v>
+        <v>137</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>166</v>
+        <v>138</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>174</v>
+        <v>146</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>163</v>
+        <v>135</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2763,7 +2723,7 @@
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4" t="s">
-        <v>167</v>
+        <v>139</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
@@ -2773,7 +2733,7 @@
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4" t="s">
-        <v>168</v>
+        <v>140</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
@@ -2783,103 +2743,103 @@
         <v>32</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B30" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B31" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="13"/>
       <c r="B33" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2887,48 +2847,48 @@
         <v>33</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>139</v>
+        <v>118</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="4" t="s">
-        <v>159</v>
+        <v>131</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="4" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>167</v>
+        <v>139</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4" t="s">
-        <v>163</v>
+        <v>135</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4" t="s">
-        <v>165</v>
+        <v>137</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>168</v>
+        <v>140</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
@@ -2938,7 +2898,7 @@
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4" t="s">
-        <v>161</v>
+        <v>133</v>
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
@@ -2948,37 +2908,37 @@
         <v>34</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>139</v>
+        <v>118</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>161</v>
+        <v>133</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="4" t="s">
-        <v>160</v>
+        <v>132</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>175</v>
+        <v>147</v>
       </c>
       <c r="G39" s="4"/>
     </row>
@@ -2986,10 +2946,10 @@
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4" t="s">
-        <v>165</v>
+        <v>137</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
@@ -3007,46 +2967,46 @@
         <v>35</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C42" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="F42" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="D42" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="E42" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="F42" s="8" t="s">
-        <v>116</v>
-      </c>
       <c r="G42" s="8" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="D43" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F43" s="4" t="s">
         <v>96</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>108</v>
       </c>
       <c r="G43" s="4"/>
     </row>
     <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="4"/>
       <c r="C44" s="4" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -3063,51 +3023,51 @@
     </row>
     <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C46" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="F46" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="D46" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="E46" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="F46" s="8" t="s">
-        <v>116</v>
-      </c>
       <c r="G46" s="9" t="s">
-        <v>164</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="4" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="G47" s="4"/>
     </row>
     <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
@@ -3124,42 +3084,42 @@
     </row>
     <row r="50" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="G50" s="9" t="s">
-        <v>162</v>
+        <v>134</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>169</v>
+        <v>141</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="G51" s="4"/>
     </row>
@@ -3169,7 +3129,7 @@
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
       <c r="F52" s="4" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="G52" s="4"/>
     </row>
@@ -3179,46 +3139,46 @@
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
       <c r="F53" s="4" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="G53" s="4"/>
     </row>
     <row r="54" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>169</v>
+        <v>141</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="G54" s="9" t="s">
-        <v>162</v>
+        <v>134</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="4"/>
       <c r="C55" s="4" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>170</v>
+        <v>142</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="G55" s="4"/>
     </row>
@@ -3240,38 +3200,38 @@
     </row>
     <row r="58" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>173</v>
+        <v>145</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>162</v>
+        <v>134</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="4" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>172</v>
+        <v>144</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="G59" s="4"/>
     </row>
@@ -3281,7 +3241,7 @@
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
       <c r="F60" s="4" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="G60" s="4"/>
     </row>
@@ -3295,22 +3255,22 @@
     </row>
     <row r="62" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>171</v>
+        <v>143</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="G62" s="8"/>
     </row>
@@ -3319,7 +3279,7 @@
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
       <c r="E63" s="4" t="s">
-        <v>172</v>
+        <v>144</v>
       </c>
       <c r="F63" s="4"/>
       <c r="G63" s="4"/>
@@ -3342,16 +3302,16 @@
     </row>
     <row r="66" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="7" t="s">
-        <v>152</v>
+        <v>124</v>
       </c>
       <c r="B66" s="8"/>
       <c r="C66" s="8"/>
       <c r="D66" s="8"/>
       <c r="E66" s="8" t="s">
-        <v>171</v>
+        <v>143</v>
       </c>
       <c r="F66" s="8" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="G66" s="8"/>
     </row>
@@ -3408,165 +3368,165 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>157</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" s="14" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
-        <v>154</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>139</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" s="14" t="s">
-        <v>153</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -3661,7 +3621,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>18</v>
@@ -3700,7 +3660,7 @@
         <v>15</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>18</v>
@@ -3741,7 +3701,7 @@
         <v>22</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>25</v>
@@ -3782,7 +3742,7 @@
         <v>23</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>27</v>
@@ -3827,7 +3787,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>31</v>
@@ -3862,73 +3822,73 @@
         <v>32</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="13"/>
       <c r="B33" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3936,7 +3896,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>40</v>
@@ -3975,7 +3935,7 @@
         <v>34</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>40</v>
@@ -3989,7 +3949,7 @@
     </row>
     <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
@@ -4024,7 +3984,7 @@
     </row>
     <row r="43" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
@@ -4044,7 +4004,7 @@
     </row>
     <row r="46" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>48</v>
@@ -4055,7 +4015,7 @@
     </row>
     <row r="47" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>

</xml_diff>